<commit_message>
Update DKMD Attendance Summer23.xlsx
</commit_message>
<xml_diff>
--- a/PMIT6307/TEST/DKMD Attendance Summer23.xlsx
+++ b/PMIT6307/TEST/DKMD Attendance Summer23.xlsx
@@ -46,15 +46,6 @@
     <t>Att (10)</t>
   </si>
   <si>
-    <t>CT1 (20)</t>
-  </si>
-  <si>
-    <t>CT2 (20)</t>
-  </si>
-  <si>
-    <t>CT3 (20)</t>
-  </si>
-  <si>
     <t>A.S. M. Sabiqul Hassan</t>
   </si>
   <si>
@@ -172,10 +163,19 @@
     <t>Assign (10)</t>
   </si>
   <si>
-    <t>Assign1 (10)</t>
-  </si>
-  <si>
-    <t>Assign2 (10)</t>
+    <t>CT1 (15)</t>
+  </si>
+  <si>
+    <t>CT2 ()</t>
+  </si>
+  <si>
+    <t>CT3 ()</t>
+  </si>
+  <si>
+    <t>Assign1 ()</t>
+  </si>
+  <si>
+    <t>Assign2 ()</t>
   </si>
 </sst>
 </file>
@@ -515,7 +515,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>5</v>
@@ -554,7 +554,7 @@
         <v>232103</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -565,7 +565,7 @@
         <v>232104</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -576,7 +576,7 @@
         <v>232105</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -587,7 +587,7 @@
         <v>232106</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -598,7 +598,7 @@
         <v>232107</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -609,7 +609,7 @@
         <v>232108</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -620,7 +620,7 @@
         <v>232109</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -631,7 +631,7 @@
         <v>232110</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -642,7 +642,7 @@
         <v>232111</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -653,7 +653,7 @@
         <v>232112</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -664,7 +664,7 @@
         <v>232113</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -675,7 +675,7 @@
         <v>232114</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -686,7 +686,7 @@
         <v>232115</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -697,7 +697,7 @@
         <v>232116</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -708,7 +708,7 @@
         <v>232117</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -719,7 +719,7 @@
         <v>232118</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -730,7 +730,7 @@
         <v>232119</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -741,7 +741,7 @@
         <v>232120</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -752,7 +752,7 @@
         <v>232121</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -763,7 +763,7 @@
         <v>232122</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -774,7 +774,7 @@
         <v>232123</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -785,7 +785,7 @@
         <v>232124</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -796,7 +796,7 @@
         <v>232125</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -807,7 +807,7 @@
         <v>232126</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -818,7 +818,7 @@
         <v>232127</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -829,7 +829,7 @@
         <v>232128</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -840,7 +840,7 @@
         <v>232129</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -851,7 +851,7 @@
         <v>232130</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -862,7 +862,7 @@
         <v>232131</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -873,7 +873,7 @@
         <v>232132</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -884,7 +884,7 @@
         <v>232133</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -895,7 +895,7 @@
         <v>232134</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -906,7 +906,7 @@
         <v>232135</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -950,7 +950,7 @@
         <v>232139</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -961,7 +961,7 @@
         <v>232140</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -979,7 +979,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>5</v>
@@ -991,16 +991,16 @@
         <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>50</v>
@@ -1009,10 +1009,10 @@
         <v>51</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -1060,7 +1060,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2">
-        <v>7</v>
+        <v>4.66</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -1068,7 +1068,7 @@
         <v>0</v>
       </c>
       <c r="L3" s="2">
-        <v>7</v>
+        <v>4.66</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1079,7 +1079,7 @@
         <v>232103</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2">
@@ -1088,7 +1088,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -1096,7 +1096,7 @@
         <v>0</v>
       </c>
       <c r="L4" s="2">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1107,7 +1107,7 @@
         <v>232104</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2">
@@ -1116,7 +1116,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2">
-        <v>5</v>
+        <v>3.33</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -1124,7 +1124,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="2">
-        <v>5</v>
+        <v>3.33</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1135,7 +1135,7 @@
         <v>232105</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2">
@@ -1144,7 +1144,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -1152,7 +1152,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1163,7 +1163,7 @@
         <v>232106</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2">
@@ -1172,7 +1172,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2">
-        <v>7</v>
+        <v>4.66</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -1180,7 +1180,7 @@
         <v>0</v>
       </c>
       <c r="L7" s="2">
-        <v>7</v>
+        <v>4.66</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1191,7 +1191,7 @@
         <v>232107</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2">
@@ -1200,7 +1200,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2">
-        <v>5</v>
+        <v>3.33</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -1208,7 +1208,7 @@
         <v>0</v>
       </c>
       <c r="L8" s="2">
-        <v>5</v>
+        <v>3.33</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1219,7 +1219,7 @@
         <v>232108</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2">
@@ -1228,7 +1228,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2">
-        <v>11</v>
+        <v>7.33</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -1236,7 +1236,7 @@
         <v>0</v>
       </c>
       <c r="L9" s="2">
-        <v>11</v>
+        <v>7.33</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1247,7 +1247,7 @@
         <v>232109</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2">
@@ -1256,7 +1256,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -1264,7 +1264,7 @@
         <v>0</v>
       </c>
       <c r="L10" s="2">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1275,7 +1275,7 @@
         <v>232110</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2">
@@ -1284,7 +1284,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2">
-        <v>10</v>
+        <v>6.66</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -1292,7 +1292,7 @@
         <v>0</v>
       </c>
       <c r="L11" s="2">
-        <v>10</v>
+        <v>6.66</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1303,7 +1303,7 @@
         <v>232111</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2">
@@ -1312,7 +1312,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2">
-        <v>5</v>
+        <v>3.33</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -1320,7 +1320,7 @@
         <v>0</v>
       </c>
       <c r="L12" s="2">
-        <v>5</v>
+        <v>3.33</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1331,7 +1331,7 @@
         <v>232112</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2">
@@ -1340,7 +1340,7 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2">
-        <v>14</v>
+        <v>9.33</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -1348,7 +1348,7 @@
         <v>0</v>
       </c>
       <c r="L13" s="2">
-        <v>14</v>
+        <v>9.33</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1359,7 +1359,7 @@
         <v>232113</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2">
@@ -1368,7 +1368,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -1376,7 +1376,7 @@
         <v>0</v>
       </c>
       <c r="L14" s="2">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1387,7 +1387,7 @@
         <v>232114</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2">
@@ -1396,7 +1396,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2">
-        <v>11</v>
+        <v>7.33</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -1404,7 +1404,7 @@
         <v>0</v>
       </c>
       <c r="L15" s="2">
-        <v>11</v>
+        <v>7.33</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1415,7 +1415,7 @@
         <v>232115</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2">
@@ -1424,7 +1424,7 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -1432,7 +1432,7 @@
         <v>0</v>
       </c>
       <c r="L16" s="2">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1443,7 +1443,7 @@
         <v>232116</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2">
@@ -1452,7 +1452,7 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2">
-        <v>5</v>
+        <v>3.33</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -1460,7 +1460,7 @@
         <v>0</v>
       </c>
       <c r="L17" s="2">
-        <v>5</v>
+        <v>3.33</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1471,7 +1471,7 @@
         <v>232117</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2">
@@ -1480,7 +1480,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2">
-        <v>8</v>
+        <v>5.33</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -1488,7 +1488,7 @@
         <v>0</v>
       </c>
       <c r="L18" s="2">
-        <v>8</v>
+        <v>5.33</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -1499,7 +1499,7 @@
         <v>232118</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2">
@@ -1527,7 +1527,7 @@
         <v>232119</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2">
@@ -1536,7 +1536,7 @@
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -1544,7 +1544,7 @@
         <v>0</v>
       </c>
       <c r="L20" s="2">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -1555,7 +1555,7 @@
         <v>232120</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2">
@@ -1564,7 +1564,7 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -1572,7 +1572,7 @@
         <v>0</v>
       </c>
       <c r="L21" s="2">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -1583,7 +1583,7 @@
         <v>232121</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2">
@@ -1592,7 +1592,7 @@
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2">
-        <v>8</v>
+        <v>5.33</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
@@ -1600,7 +1600,7 @@
         <v>0</v>
       </c>
       <c r="L22" s="2">
-        <v>8</v>
+        <v>5.33</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -1611,7 +1611,7 @@
         <v>232122</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2">
@@ -1620,7 +1620,7 @@
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2">
-        <v>4</v>
+        <v>2.66</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
@@ -1628,7 +1628,7 @@
         <v>0</v>
       </c>
       <c r="L23" s="2">
-        <v>4</v>
+        <v>2.66</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -1639,7 +1639,7 @@
         <v>232123</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2">
@@ -1648,7 +1648,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2">
-        <v>7</v>
+        <v>4.66</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -1656,7 +1656,7 @@
         <v>0</v>
       </c>
       <c r="L24" s="2">
-        <v>7</v>
+        <v>4.66</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -1667,7 +1667,7 @@
         <v>232124</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2">
@@ -1676,7 +1676,7 @@
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2">
-        <v>11</v>
+        <v>7.33</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
@@ -1684,7 +1684,7 @@
         <v>0</v>
       </c>
       <c r="L25" s="2">
-        <v>11</v>
+        <v>7.33</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -1695,7 +1695,7 @@
         <v>232125</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2">
@@ -1704,7 +1704,7 @@
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2">
-        <v>13</v>
+        <v>8.66</v>
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
@@ -1712,7 +1712,7 @@
         <v>0</v>
       </c>
       <c r="L26" s="2">
-        <v>13</v>
+        <v>8.66</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -1723,7 +1723,7 @@
         <v>232126</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2">
@@ -1732,7 +1732,7 @@
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2">
-        <v>10</v>
+        <v>6.66</v>
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
@@ -1740,7 +1740,7 @@
         <v>0</v>
       </c>
       <c r="L27" s="2">
-        <v>10</v>
+        <v>6.66</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -1751,7 +1751,7 @@
         <v>232127</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2">
@@ -1760,7 +1760,7 @@
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2">
-        <v>7</v>
+        <v>4.66</v>
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
@@ -1768,7 +1768,7 @@
         <v>0</v>
       </c>
       <c r="L28" s="2">
-        <v>7</v>
+        <v>4.66</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -1779,7 +1779,7 @@
         <v>232128</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2">
@@ -1788,7 +1788,7 @@
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2">
-        <v>7</v>
+        <v>4.66</v>
       </c>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
@@ -1796,7 +1796,7 @@
         <v>0</v>
       </c>
       <c r="L29" s="2">
-        <v>7</v>
+        <v>4.66</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -1807,7 +1807,7 @@
         <v>232129</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2">
@@ -1816,7 +1816,7 @@
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2">
-        <v>11</v>
+        <v>7.33</v>
       </c>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
@@ -1824,7 +1824,7 @@
         <v>0</v>
       </c>
       <c r="L30" s="2">
-        <v>11</v>
+        <v>7.33</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -1835,7 +1835,7 @@
         <v>232130</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2">
@@ -1844,7 +1844,7 @@
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
@@ -1852,7 +1852,7 @@
         <v>0</v>
       </c>
       <c r="L31" s="2">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -1863,7 +1863,7 @@
         <v>232131</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2">
@@ -1872,7 +1872,7 @@
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2">
-        <v>7</v>
+        <v>4.66</v>
       </c>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
@@ -1880,7 +1880,7 @@
         <v>0</v>
       </c>
       <c r="L32" s="2">
-        <v>7</v>
+        <v>4.66</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -1891,7 +1891,7 @@
         <v>232132</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2">
@@ -1900,7 +1900,7 @@
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2">
-        <v>5</v>
+        <v>3.33</v>
       </c>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
@@ -1908,7 +1908,7 @@
         <v>0</v>
       </c>
       <c r="L33" s="2">
-        <v>5</v>
+        <v>3.33</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -1919,7 +1919,7 @@
         <v>232133</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2">
@@ -1928,7 +1928,7 @@
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2">
-        <v>10</v>
+        <v>6.66</v>
       </c>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
@@ -1936,7 +1936,7 @@
         <v>0</v>
       </c>
       <c r="L34" s="2">
-        <v>10</v>
+        <v>6.66</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -1947,7 +1947,7 @@
         <v>232134</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2">
@@ -1956,7 +1956,7 @@
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2">
-        <v>8</v>
+        <v>5.33</v>
       </c>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
@@ -1964,7 +1964,7 @@
         <v>0</v>
       </c>
       <c r="L35" s="2">
-        <v>8</v>
+        <v>5.33</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -1975,7 +1975,7 @@
         <v>232135</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2">
@@ -1984,7 +1984,7 @@
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
@@ -1992,7 +1992,7 @@
         <v>0</v>
       </c>
       <c r="L36" s="2">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -2012,7 +2012,7 @@
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2">
-        <v>11</v>
+        <v>7.33</v>
       </c>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
@@ -2020,7 +2020,7 @@
         <v>0</v>
       </c>
       <c r="L37" s="2">
-        <v>11</v>
+        <v>7.33</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -2040,7 +2040,7 @@
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
@@ -2048,7 +2048,7 @@
         <v>0</v>
       </c>
       <c r="L38" s="2">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -2068,7 +2068,7 @@
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2">
-        <v>5</v>
+        <v>3.33</v>
       </c>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
@@ -2076,7 +2076,7 @@
         <v>0</v>
       </c>
       <c r="L39" s="2">
-        <v>5</v>
+        <v>3.33</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -2087,7 +2087,7 @@
         <v>232139</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2">
@@ -2096,7 +2096,7 @@
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2">
-        <v>7</v>
+        <v>4.66</v>
       </c>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
@@ -2104,7 +2104,7 @@
         <v>0</v>
       </c>
       <c r="L40" s="2">
-        <v>7</v>
+        <v>4.66</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
@@ -2115,7 +2115,7 @@
         <v>232140</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2">
@@ -2124,7 +2124,7 @@
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2">
-        <v>10</v>
+        <v>6.66</v>
       </c>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
@@ -2132,10 +2132,13 @@
         <v>0</v>
       </c>
       <c r="L41" s="2">
-        <v>10</v>
+        <v>6.66</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:L41">
+    <sortCondition ref="A1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>